<commit_message>
TX - completed all data migration scripts.  Data ready for import into WaDE
</commit_message>
<xml_diff>
--- a/Texas/WaterAllocation/TX_Allocation Schema Mapping to WaDE_QA.xlsx
+++ b/Texas/WaterAllocation/TX_Allocation Schema Mapping to WaDE_QA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/augustus/Desktop/WSWC/WaDE/MappingStatesDataToWaDE2.0/Texas/WaterAllocation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BB68FF75-0C12-6942-B0ED-EAFC96B0D3FE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7275958D-3202-F847-913D-B6039AA7F75B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6440" yWindow="2660" windowWidth="30940" windowHeight="16900" tabRatio="714" activeTab="1" xr2:uid="{10FC1BAB-5472-410C-A2F0-85DCDF5389F8}"/>
+    <workbookView xWindow="1520" yWindow="460" windowWidth="37200" windowHeight="18240" tabRatio="714" activeTab="5" xr2:uid="{10FC1BAB-5472-410C-A2F0-85DCDF5389F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapping Notes" sheetId="10" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="277">
   <si>
     <t>AllocationAmount</t>
   </si>
@@ -525,9 +525,54 @@
     <t>State WFS Field Name</t>
   </si>
   <si>
+    <t>TCEQ _Water Rights</t>
+  </si>
+  <si>
+    <t>Surface Ground</t>
+  </si>
+  <si>
+    <t>(blank)</t>
+  </si>
+  <si>
+    <t>Water Rights</t>
+  </si>
+  <si>
+    <t>Texas Water Rights</t>
+  </si>
+  <si>
+    <t>TCEQ_Allocation all</t>
+  </si>
+  <si>
+    <t>AF</t>
+  </si>
+  <si>
+    <t>TCEQ</t>
+  </si>
+  <si>
+    <t>https://www.tceq.texas.gov/permitting/water_rights/wr-permitting/wrwud</t>
+  </si>
+  <si>
+    <t>TX</t>
+  </si>
+  <si>
+    <t>Texas Commission on Environmental Quality</t>
+  </si>
+  <si>
+    <t>512-239-1000</t>
+  </si>
+  <si>
+    <t>The Texas Commission on Environmental Quality is the environmental agency for the state.</t>
+  </si>
+  <si>
+    <t>https://www.tceq.texas.gov/</t>
+  </si>
+  <si>
     <t>?</t>
   </si>
   <si>
+    <t>These are in NAD83 (Project to WGS84)</t>
+  </si>
+  <si>
     <t>Internal unique identifier integer</t>
   </si>
   <si>
@@ -726,6 +771,9 @@
     <t>From a map? GPS? Where coordinate from? Full list available at: http://vocabulary.westernstateswater.org/coordinatemethod/.  Append if needed.</t>
   </si>
   <si>
+    <t>Use</t>
+  </si>
+  <si>
     <t>Whether or not the point location is indexed to the USGS NHD network.  List available at: http://vocabulary.westernstateswater.org/nhdnetworkstatus/.  Append if needed.</t>
   </si>
   <si>
@@ -762,19 +810,64 @@
     <t>State:</t>
   </si>
   <si>
+    <t>Texas</t>
+  </si>
+  <si>
     <t>Organizaitons:</t>
   </si>
   <si>
     <t>Data Links:</t>
   </si>
   <si>
+    <t>https://www.tceq.texas.gov/permitting/water_rights</t>
+  </si>
+  <si>
+    <t>https://tceq.maps.arcgis.com/home/item.html?id=796b001513b9407a9818897b4dc1ec4d</t>
+  </si>
+  <si>
     <t>Notes:</t>
   </si>
   <si>
-    <t>Texas</t>
-  </si>
-  <si>
-    <t>Texas Commission on Environmental Quality</t>
+    <t>Estimated</t>
+  </si>
+  <si>
+    <t>john-cody.stalsby@tceq.texas.gov</t>
+  </si>
+  <si>
+    <t>John-Cody Stalsby</t>
+  </si>
+  <si>
+    <t>"TCEQ_" + counter starting at 1</t>
+  </si>
+  <si>
+    <t>Water Right ID</t>
+  </si>
+  <si>
+    <t>OWN_NAME</t>
+  </si>
+  <si>
+    <t>TYPE (Water Right Point)</t>
+  </si>
+  <si>
+    <t>LONG_DD (Water Right Point)</t>
+  </si>
+  <si>
+    <t>LAT_DD (Water Right Point)</t>
+  </si>
+  <si>
+    <t>TCEQ_ID</t>
+  </si>
+  <si>
+    <t>EPSG: 4269</t>
+  </si>
+  <si>
+    <t>TCEQ _WaterRights</t>
+  </si>
+  <si>
+    <t>Use dummy row</t>
+  </si>
+  <si>
+    <t>"TX_" + counter starting at 1</t>
   </si>
 </sst>
 </file>
@@ -784,7 +877,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d;@"/>
   </numFmts>
-  <fonts count="31" x14ac:knownFonts="1">
+  <fonts count="30" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1008,13 +1101,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -1203,7 +1289,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -1482,6 +1568,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1528,7 +1634,7 @@
     <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1713,12 +1819,6 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="23" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1768,10 +1868,22 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="21" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="25" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="18" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="23" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2133,48 +2245,56 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.5" style="80" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5" style="78" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="79" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="80" t="s">
-        <v>240</v>
+      <c r="A1" s="78" t="s">
+        <v>256</v>
       </c>
       <c r="B1" t="s">
-        <v>244</v>
+        <v>257</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="80" t="s">
-        <v>241</v>
+      <c r="A2" s="78" t="s">
+        <v>258</v>
       </c>
       <c r="B2" t="s">
-        <v>245</v>
+        <v>172</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="80" t="s">
-        <v>242</v>
+      <c r="A6" s="78" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B7" s="69"/>
+      <c r="B7" s="67" t="s">
+        <v>260</v>
+      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B8" s="69"/>
+      <c r="B8" s="67" t="s">
+        <v>261</v>
+      </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="80" t="s">
-        <v>243</v>
+      <c r="A13" s="78" t="s">
+        <v>262</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B7" r:id="rId1" xr:uid="{B9D02653-C6FC-45DD-931D-0F09F93B6279}"/>
+    <hyperlink ref="B8" r:id="rId2" xr:uid="{E2B15040-D3FE-4D7D-83F1-F635828A9462}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2183,8 +2303,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2606DDD-D901-4365-BB8D-3E6142C84460}">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2269,8 +2389,8 @@
       <c r="I3" s="17">
         <v>11</v>
       </c>
-      <c r="J3" s="71" t="s">
-        <v>173</v>
+      <c r="J3" s="69" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -2286,7 +2406,9 @@
       <c r="D4" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="E4" s="64"/>
+      <c r="E4" s="62" t="s">
+        <v>162</v>
+      </c>
       <c r="F4" s="46"/>
       <c r="G4" s="47"/>
       <c r="H4" s="9" t="s">
@@ -2295,8 +2417,8 @@
       <c r="I4" s="17" t="s">
         <v>141</v>
       </c>
-      <c r="J4" s="71" t="s">
-        <v>192</v>
+      <c r="J4" s="69" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="36" x14ac:dyDescent="0.2">
@@ -2312,7 +2434,9 @@
       <c r="D5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="18"/>
+      <c r="E5" s="18" t="s">
+        <v>163</v>
+      </c>
       <c r="F5" s="20"/>
       <c r="G5" s="21"/>
       <c r="H5" s="9" t="s">
@@ -2321,8 +2445,8 @@
       <c r="I5" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="J5" s="71" t="s">
-        <v>218</v>
+      <c r="J5" s="69" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -2338,17 +2462,19 @@
       <c r="D6" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E6" s="20"/>
+      <c r="E6" s="20" t="s">
+        <v>164</v>
+      </c>
       <c r="F6" s="20"/>
       <c r="G6" s="21"/>
       <c r="H6" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="I6" s="79">
+      <c r="I6" s="77">
         <v>0.5</v>
       </c>
-      <c r="J6" s="71" t="s">
-        <v>175</v>
+      <c r="J6" s="69" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -2364,7 +2490,9 @@
       <c r="D7" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E7" s="20"/>
+      <c r="E7" s="20" t="s">
+        <v>164</v>
+      </c>
       <c r="F7" s="20"/>
       <c r="G7" s="21"/>
       <c r="H7" s="9" t="s">
@@ -2373,8 +2501,8 @@
       <c r="I7" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="J7" s="71" t="s">
-        <v>174</v>
+      <c r="J7" s="69" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="24" x14ac:dyDescent="0.2">
@@ -2390,17 +2518,19 @@
       <c r="D8" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="20"/>
+      <c r="E8" s="20" t="s">
+        <v>164</v>
+      </c>
       <c r="F8" s="20"/>
       <c r="G8" s="21"/>
       <c r="H8" s="9" t="s">
         <v>39</v>
       </c>
       <c r="I8" s="20" t="s">
-        <v>214</v>
-      </c>
-      <c r="J8" s="71" t="s">
-        <v>220</v>
+        <v>229</v>
+      </c>
+      <c r="J8" s="69" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -2416,15 +2546,17 @@
       <c r="D9" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E9" s="18"/>
+      <c r="E9" s="18" t="s">
+        <v>165</v>
+      </c>
       <c r="F9" s="20"/>
       <c r="G9" s="21"/>
       <c r="H9" s="9" t="s">
         <v>39</v>
       </c>
       <c r="I9" s="18"/>
-      <c r="J9" s="71" t="s">
-        <v>215</v>
+      <c r="J9" s="69" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
@@ -2440,7 +2572,9 @@
       <c r="D10" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="18"/>
+      <c r="E10" s="18" t="s">
+        <v>166</v>
+      </c>
       <c r="F10" s="20"/>
       <c r="G10" s="21"/>
       <c r="H10" s="9" t="s">
@@ -2449,11 +2583,11 @@
       <c r="I10" s="17" t="s">
         <v>145</v>
       </c>
-      <c r="J10" s="71" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J10" s="69" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="39" x14ac:dyDescent="0.15">
       <c r="A11" s="5" t="s">
         <v>10</v>
       </c>
@@ -2466,7 +2600,9 @@
       <c r="D11" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E11" s="18"/>
+      <c r="E11" s="79" t="s">
+        <v>261</v>
+      </c>
       <c r="F11" s="20"/>
       <c r="G11" s="21"/>
       <c r="H11" s="9" t="s">
@@ -2475,8 +2611,8 @@
       <c r="I11" s="17" t="s">
         <v>109</v>
       </c>
-      <c r="J11" s="71" t="s">
-        <v>176</v>
+      <c r="J11" s="69" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="24" x14ac:dyDescent="0.2">
@@ -2492,7 +2628,9 @@
       <c r="D12" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="20"/>
+      <c r="E12" s="20" t="s">
+        <v>263</v>
+      </c>
       <c r="F12" s="20"/>
       <c r="G12" s="21"/>
       <c r="H12" s="9" t="s">
@@ -2501,8 +2639,8 @@
       <c r="I12" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="J12" s="71" t="s">
-        <v>219</v>
+      <c r="J12" s="69" t="s">
+        <v>234</v>
       </c>
     </row>
   </sheetData>
@@ -2519,7 +2657,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2589,17 +2727,23 @@
       <c r="D3" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="34"/>
+      <c r="E3" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" s="34" t="s">
+        <v>39</v>
+      </c>
       <c r="H3" s="9" t="s">
         <v>39</v>
       </c>
       <c r="I3" s="17">
         <v>16</v>
       </c>
-      <c r="J3" s="71" t="s">
-        <v>173</v>
+      <c r="J3" s="69" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -2615,17 +2759,23 @@
       <c r="D4" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="47"/>
+      <c r="E4" s="46" t="s">
+        <v>167</v>
+      </c>
+      <c r="F4" s="46" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" s="47" t="s">
+        <v>39</v>
+      </c>
       <c r="H4" s="9" t="s">
         <v>39</v>
       </c>
       <c r="I4" s="17" t="s">
         <v>142</v>
       </c>
-      <c r="J4" s="71" t="s">
-        <v>177</v>
+      <c r="J4" s="69" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="24" x14ac:dyDescent="0.2">
@@ -2641,7 +2791,9 @@
       <c r="D5" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E5" s="17"/>
+      <c r="E5" s="17">
+        <v>1</v>
+      </c>
       <c r="F5" s="20"/>
       <c r="G5" s="21"/>
       <c r="H5" s="9" t="s">
@@ -2650,8 +2802,8 @@
       <c r="I5" s="17">
         <v>1</v>
       </c>
-      <c r="J5" s="71" t="s">
-        <v>178</v>
+      <c r="J5" s="69" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -2667,7 +2819,9 @@
       <c r="D6" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="17"/>
+      <c r="E6" s="17" t="s">
+        <v>113</v>
+      </c>
       <c r="F6" s="20"/>
       <c r="G6" s="21"/>
       <c r="H6" s="9" t="s">
@@ -2676,8 +2830,8 @@
       <c r="I6" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="J6" s="71" t="s">
-        <v>179</v>
+      <c r="J6" s="69" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -2693,7 +2847,9 @@
       <c r="D7" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="17"/>
+      <c r="E7" s="17" t="s">
+        <v>112</v>
+      </c>
       <c r="F7" s="20"/>
       <c r="G7" s="21"/>
       <c r="H7" s="9" t="s">
@@ -2702,8 +2858,8 @@
       <c r="I7" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="J7" s="71" t="s">
-        <v>221</v>
+      <c r="J7" s="69" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
@@ -2719,7 +2875,9 @@
       <c r="D8" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="17"/>
+      <c r="E8" s="17" t="s">
+        <v>115</v>
+      </c>
       <c r="F8" s="20"/>
       <c r="G8" s="21"/>
       <c r="H8" s="9" t="s">
@@ -2728,8 +2886,8 @@
       <c r="I8" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="J8" s="71" t="s">
-        <v>222</v>
+      <c r="J8" s="69" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -2745,7 +2903,9 @@
       <c r="D9" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="17"/>
+      <c r="E9" s="17" t="s">
+        <v>168</v>
+      </c>
       <c r="F9" s="20"/>
       <c r="G9" s="21"/>
       <c r="H9" s="9" t="s">
@@ -2754,8 +2914,8 @@
       <c r="I9" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="J9" s="71" t="s">
-        <v>216</v>
+      <c r="J9" s="69" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
@@ -2771,7 +2931,9 @@
       <c r="D10" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="17"/>
+      <c r="E10" s="17">
+        <v>10</v>
+      </c>
       <c r="F10" s="20"/>
       <c r="G10" s="21"/>
       <c r="H10" s="9" t="s">
@@ -2780,8 +2942,8 @@
       <c r="I10" s="17">
         <v>10</v>
       </c>
-      <c r="J10" s="71" t="s">
-        <v>180</v>
+      <c r="J10" s="69" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="24" x14ac:dyDescent="0.2">
@@ -2797,7 +2959,9 @@
       <c r="D11" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="17"/>
+      <c r="E11" s="17" t="s">
+        <v>114</v>
+      </c>
       <c r="F11" s="20"/>
       <c r="G11" s="21"/>
       <c r="H11" s="9" t="s">
@@ -2806,8 +2970,8 @@
       <c r="I11" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="J11" s="71" t="s">
-        <v>223</v>
+      <c r="J11" s="69" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="24" x14ac:dyDescent="0.2">
@@ -2823,7 +2987,9 @@
       <c r="D12" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="17"/>
+      <c r="E12" s="17" t="s">
+        <v>146</v>
+      </c>
       <c r="F12" s="20"/>
       <c r="G12" s="21"/>
       <c r="H12" s="9" t="s">
@@ -2832,8 +2998,8 @@
       <c r="I12" s="17" t="s">
         <v>146</v>
       </c>
-      <c r="J12" s="71" t="s">
-        <v>224</v>
+      <c r="J12" s="69" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="48" x14ac:dyDescent="0.2">
@@ -2849,7 +3015,9 @@
       <c r="D13" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="17"/>
+      <c r="E13" s="17" t="s">
+        <v>117</v>
+      </c>
       <c r="F13" s="20"/>
       <c r="G13" s="21"/>
       <c r="H13" s="9" t="s">
@@ -2858,8 +3026,8 @@
       <c r="I13" s="17" t="s">
         <v>117</v>
       </c>
-      <c r="J13" s="71" t="s">
-        <v>217</v>
+      <c r="J13" s="69" t="s">
+        <v>232</v>
       </c>
     </row>
   </sheetData>
@@ -2875,8 +3043,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E8BA2FE-2555-4166-A4DF-0203EE1C77D7}">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4:G12"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2961,8 +3129,8 @@
       <c r="I3" s="18">
         <v>1</v>
       </c>
-      <c r="J3" s="71" t="s">
-        <v>173</v>
+      <c r="J3" s="69" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -2978,20 +3146,26 @@
       <c r="D4" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="E4" s="44"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="47"/>
+      <c r="E4" s="44" t="s">
+        <v>169</v>
+      </c>
+      <c r="F4" s="46" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" s="47" t="s">
+        <v>39</v>
+      </c>
       <c r="H4" s="9" t="s">
         <v>39</v>
       </c>
       <c r="I4" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="J4" s="71" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J4" s="69" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="26" x14ac:dyDescent="0.15">
       <c r="A5" s="5" t="s">
         <v>79</v>
       </c>
@@ -3004,7 +3178,9 @@
       <c r="D5" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E5" s="18"/>
+      <c r="E5" s="79" t="s">
+        <v>264</v>
+      </c>
       <c r="F5" s="20"/>
       <c r="G5" s="21"/>
       <c r="H5" s="9" t="s">
@@ -3013,8 +3189,8 @@
       <c r="I5" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="J5" s="71" t="s">
-        <v>182</v>
+      <c r="J5" s="69" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -3030,7 +3206,9 @@
       <c r="D6" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E6" s="18"/>
+      <c r="E6" s="18" t="s">
+        <v>265</v>
+      </c>
       <c r="F6" s="20"/>
       <c r="G6" s="21"/>
       <c r="H6" s="9" t="s">
@@ -3039,11 +3217,11 @@
       <c r="I6" s="18" t="s">
         <v>131</v>
       </c>
-      <c r="J6" s="71" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="26" x14ac:dyDescent="0.2">
+      <c r="J6" s="69" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="39" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>80</v>
       </c>
@@ -3056,7 +3234,9 @@
       <c r="D7" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E7" s="18"/>
+      <c r="E7" s="18" t="s">
+        <v>170</v>
+      </c>
       <c r="F7" s="20"/>
       <c r="G7" s="21"/>
       <c r="H7" s="9" t="s">
@@ -3065,11 +3245,11 @@
       <c r="I7" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="J7" s="71" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J7" s="69" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="26" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>74</v>
       </c>
@@ -3082,7 +3262,9 @@
       <c r="D8" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E8" s="18"/>
+      <c r="E8" s="18" t="s">
+        <v>172</v>
+      </c>
       <c r="F8" s="20"/>
       <c r="G8" s="21"/>
       <c r="H8" s="9" t="s">
@@ -3091,8 +3273,8 @@
       <c r="I8" s="18" t="s">
         <v>149</v>
       </c>
-      <c r="J8" s="71" t="s">
-        <v>185</v>
+      <c r="J8" s="69" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -3108,7 +3290,9 @@
       <c r="D9" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E9" s="18"/>
+      <c r="E9" s="18" t="s">
+        <v>173</v>
+      </c>
       <c r="F9" s="20"/>
       <c r="G9" s="21"/>
       <c r="H9" s="9" t="s">
@@ -3117,11 +3301,11 @@
       <c r="I9" s="18" t="s">
         <v>130</v>
       </c>
-      <c r="J9" s="71" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J9" s="69" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="52" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>75</v>
       </c>
@@ -3134,7 +3318,9 @@
       <c r="D10" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="18"/>
+      <c r="E10" s="18" t="s">
+        <v>174</v>
+      </c>
       <c r="F10" s="20"/>
       <c r="G10" s="21"/>
       <c r="H10" s="9" t="s">
@@ -3143,8 +3329,8 @@
       <c r="I10" s="18" t="s">
         <v>150</v>
       </c>
-      <c r="J10" s="71" t="s">
-        <v>187</v>
+      <c r="J10" s="69" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="26" x14ac:dyDescent="0.2">
@@ -3160,7 +3346,9 @@
       <c r="D11" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E11" s="18"/>
+      <c r="E11" s="18" t="s">
+        <v>175</v>
+      </c>
       <c r="F11" s="20"/>
       <c r="G11" s="21"/>
       <c r="H11" s="9" t="s">
@@ -3169,8 +3357,8 @@
       <c r="I11" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="J11" s="71" t="s">
-        <v>188</v>
+      <c r="J11" s="69" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
@@ -3186,7 +3374,9 @@
       <c r="D12" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E12" s="18"/>
+      <c r="E12" s="18" t="s">
+        <v>171</v>
+      </c>
       <c r="F12" s="20"/>
       <c r="G12" s="21"/>
       <c r="H12" s="9" t="s">
@@ -3195,8 +3385,8 @@
       <c r="I12" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="J12" s="71" t="s">
-        <v>189</v>
+      <c r="J12" s="69" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
@@ -3237,7 +3427,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4:G10"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3320,8 +3510,8 @@
       <c r="I3" s="17">
         <v>34658</v>
       </c>
-      <c r="J3" s="71" t="s">
-        <v>173</v>
+      <c r="J3" s="69" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -3337,15 +3527,17 @@
       <c r="D4" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="E4" s="50"/>
+      <c r="E4" s="50" t="s">
+        <v>276</v>
+      </c>
       <c r="F4" s="46"/>
       <c r="G4" s="49"/>
       <c r="H4" s="19"/>
       <c r="I4" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="J4" s="71" t="s">
-        <v>191</v>
+      <c r="J4" s="69" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="36" x14ac:dyDescent="0.2">
@@ -3361,15 +3553,17 @@
       <c r="D5" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E5" s="81"/>
+      <c r="E5" s="68" t="s">
+        <v>176</v>
+      </c>
       <c r="F5" s="22"/>
       <c r="G5" s="21"/>
       <c r="H5" s="19"/>
       <c r="I5" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="J5" s="71" t="s">
-        <v>165</v>
+      <c r="J5" s="69" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="36" x14ac:dyDescent="0.2">
@@ -3385,15 +3579,17 @@
       <c r="D6" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="81"/>
+      <c r="E6" s="68" t="s">
+        <v>176</v>
+      </c>
       <c r="F6" s="22"/>
       <c r="G6" s="21"/>
       <c r="H6" s="19"/>
       <c r="I6" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="J6" s="71" t="s">
-        <v>225</v>
+      <c r="J6" s="69" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="36" x14ac:dyDescent="0.2">
@@ -3409,15 +3605,17 @@
       <c r="D7" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="20"/>
+      <c r="E7" s="20" t="s">
+        <v>120</v>
+      </c>
       <c r="F7" s="22"/>
       <c r="G7" s="21"/>
       <c r="H7" s="19"/>
       <c r="I7" s="17" t="s">
         <v>120</v>
       </c>
-      <c r="J7" s="71" t="s">
-        <v>226</v>
+      <c r="J7" s="69" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
@@ -3433,15 +3631,17 @@
       <c r="D8" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E8" s="82"/>
+      <c r="E8" s="68" t="s">
+        <v>176</v>
+      </c>
       <c r="F8" s="22"/>
       <c r="G8" s="21"/>
       <c r="H8" s="23"/>
       <c r="I8" s="17" t="s">
-        <v>190</v>
-      </c>
-      <c r="J8" s="71" t="s">
-        <v>193</v>
+        <v>205</v>
+      </c>
+      <c r="J8" s="69" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -3457,15 +3657,17 @@
       <c r="D9" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E9" s="82"/>
+      <c r="E9" s="68" t="s">
+        <v>176</v>
+      </c>
       <c r="F9" s="22"/>
       <c r="G9" s="21"/>
       <c r="H9" s="19"/>
       <c r="I9" s="17">
         <v>17839</v>
       </c>
-      <c r="J9" s="71" t="s">
-        <v>194</v>
+      <c r="J9" s="69" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="36" x14ac:dyDescent="0.2">
@@ -3481,15 +3683,17 @@
       <c r="D10" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="82"/>
+      <c r="E10" s="68" t="s">
+        <v>176</v>
+      </c>
       <c r="F10" s="60"/>
       <c r="G10" s="21"/>
       <c r="H10" s="23"/>
       <c r="I10" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="J10" s="71" t="s">
-        <v>227</v>
+      <c r="J10" s="69" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
@@ -3513,8 +3717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10E7F0DF-14BE-4BB8-BB6C-8815808B0B66}">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4:G22"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J3" sqref="J2:J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3597,8 +3801,8 @@
       <c r="I3" s="18">
         <v>39035</v>
       </c>
-      <c r="J3" s="71" t="s">
-        <v>163</v>
+      <c r="J3" s="69" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -3612,15 +3816,17 @@
       <c r="D4" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="E4" s="50"/>
+      <c r="E4" s="50" t="s">
+        <v>266</v>
+      </c>
       <c r="F4" s="46"/>
       <c r="G4" s="47"/>
       <c r="H4" s="19"/>
       <c r="I4" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="J4" s="71" t="s">
-        <v>164</v>
+      <c r="J4" s="69" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -3636,15 +3842,17 @@
       <c r="D5" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E5" s="70"/>
+      <c r="E5" s="68" t="s">
+        <v>119</v>
+      </c>
       <c r="F5" s="20"/>
       <c r="G5" s="21"/>
       <c r="H5" s="19"/>
       <c r="I5" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="J5" s="71" t="s">
-        <v>232</v>
+      <c r="J5" s="69" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="24" x14ac:dyDescent="0.2">
@@ -3660,15 +3868,17 @@
       <c r="D6" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="70"/>
+      <c r="E6" s="22" t="s">
+        <v>126</v>
+      </c>
       <c r="F6" s="26"/>
       <c r="G6" s="27"/>
       <c r="H6" s="19"/>
       <c r="I6" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="J6" s="71" t="s">
-        <v>228</v>
+      <c r="J6" s="69" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="16" x14ac:dyDescent="0.2">
@@ -3691,8 +3901,8 @@
       <c r="I7" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="J7" s="72" t="s">
-        <v>162</v>
+      <c r="J7" s="70" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
@@ -3708,15 +3918,21 @@
       <c r="D8" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="27"/>
+      <c r="E8" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="F8" s="26" t="s">
+        <v>169</v>
+      </c>
+      <c r="G8" s="27" t="s">
+        <v>273</v>
+      </c>
       <c r="H8" s="23"/>
       <c r="I8" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="J8" s="71" t="s">
-        <v>166</v>
+      <c r="J8" s="69" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="24" x14ac:dyDescent="0.2">
@@ -3737,8 +3953,8 @@
       <c r="G9" s="27"/>
       <c r="H9" s="19"/>
       <c r="I9" s="18"/>
-      <c r="J9" s="71" t="s">
-        <v>165</v>
+      <c r="J9" s="69" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="60" x14ac:dyDescent="0.2">
@@ -3761,8 +3977,8 @@
       <c r="I10" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="J10" s="71" t="s">
-        <v>167</v>
+      <c r="J10" s="69" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="16" x14ac:dyDescent="0.2">
@@ -3785,8 +4001,8 @@
       <c r="I11" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="J11" s="72" t="s">
-        <v>162</v>
+      <c r="J11" s="70" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="16" x14ac:dyDescent="0.2">
@@ -3809,8 +4025,8 @@
       <c r="I12" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="J12" s="72" t="s">
-        <v>162</v>
+      <c r="J12" s="70" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="24" x14ac:dyDescent="0.2">
@@ -3826,15 +4042,21 @@
       <c r="D13" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E13" s="26"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="21"/>
+      <c r="E13" s="26" t="s">
+        <v>177</v>
+      </c>
+      <c r="F13" s="26" t="s">
+        <v>169</v>
+      </c>
+      <c r="G13" s="21" t="s">
+        <v>271</v>
+      </c>
       <c r="H13" s="25"/>
       <c r="I13" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="J13" s="71" t="s">
-        <v>168</v>
+      <c r="J13" s="69" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="24" x14ac:dyDescent="0.2">
@@ -3850,15 +4072,21 @@
       <c r="D14" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="21"/>
+      <c r="E14" s="26" t="s">
+        <v>177</v>
+      </c>
+      <c r="F14" s="26" t="s">
+        <v>169</v>
+      </c>
+      <c r="G14" s="21" t="s">
+        <v>270</v>
+      </c>
       <c r="H14" s="25"/>
       <c r="I14" s="18">
         <v>-1067.700435</v>
       </c>
-      <c r="J14" s="71" t="s">
-        <v>169</v>
+      <c r="J14" s="69" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="24" x14ac:dyDescent="0.2">
@@ -3881,8 +4109,8 @@
       <c r="I15" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="J15" s="71" t="s">
-        <v>229</v>
+      <c r="J15" s="69" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="24" x14ac:dyDescent="0.2">
@@ -3905,8 +4133,8 @@
       <c r="I16" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="J16" s="71" t="s">
-        <v>233</v>
+      <c r="J16" s="69" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
@@ -3927,8 +4155,8 @@
       <c r="I17" s="18" t="s">
         <v>122</v>
       </c>
-      <c r="J17" s="71" t="s">
-        <v>170</v>
+      <c r="J17" s="69" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
@@ -3945,14 +4173,18 @@
         <v>39</v>
       </c>
       <c r="E18" s="26"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="21"/>
+      <c r="F18" s="26" t="s">
+        <v>169</v>
+      </c>
+      <c r="G18" s="21" t="s">
+        <v>272</v>
+      </c>
       <c r="H18" s="23"/>
       <c r="I18" s="18">
         <v>3703994</v>
       </c>
-      <c r="J18" s="71" t="s">
-        <v>171</v>
+      <c r="J18" s="69" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="26" x14ac:dyDescent="0.2">
@@ -3975,8 +4207,8 @@
       <c r="I19" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="J19" s="72" t="s">
-        <v>162</v>
+      <c r="J19" s="70" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
@@ -3993,14 +4225,18 @@
         <v>21</v>
       </c>
       <c r="E20" s="61"/>
-      <c r="F20" s="26"/>
-      <c r="G20" s="24"/>
+      <c r="F20" s="26" t="s">
+        <v>169</v>
+      </c>
+      <c r="G20" s="24" t="s">
+        <v>269</v>
+      </c>
       <c r="H20" s="19"/>
       <c r="I20" s="18" t="s">
         <v>123</v>
       </c>
-      <c r="J20" s="71" t="s">
-        <v>230</v>
+      <c r="J20" s="69" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
@@ -4016,15 +4252,17 @@
       <c r="D21" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E21" s="26"/>
+      <c r="E21" s="26" t="s">
+        <v>171</v>
+      </c>
       <c r="F21" s="26"/>
       <c r="G21" s="27"/>
       <c r="H21" s="19"/>
       <c r="I21" s="18" t="s">
         <v>143</v>
       </c>
-      <c r="J21" s="71" t="s">
-        <v>231</v>
+      <c r="J21" s="69" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="16" x14ac:dyDescent="0.2">
@@ -4047,8 +4285,8 @@
       <c r="I22" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="J22" s="72" t="s">
-        <v>162</v>
+      <c r="J22" s="70" t="s">
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -4064,21 +4302,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B91B1FF-D207-4871-B787-27544A9D3030}">
   <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="39.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.83203125" style="5" customWidth="1"/>
     <col min="2" max="2" width="13" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.5" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="46.83203125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="18.83203125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="34.1640625" style="5" customWidth="1"/>
-    <col min="8" max="8" width="18.1640625" style="5" customWidth="1"/>
-    <col min="9" max="9" width="23.33203125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="21.1640625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="16.33203125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="16.5" style="5" customWidth="1"/>
+    <col min="8" max="8" width="13.1640625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="20.83203125" style="5" customWidth="1"/>
     <col min="10" max="10" width="116.1640625" style="5" customWidth="1"/>
     <col min="11" max="16384" width="8.83203125" style="5"/>
   </cols>
@@ -4141,11 +4379,11 @@
       <c r="H3" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="I3" s="73">
+      <c r="I3" s="71">
         <v>50004</v>
       </c>
-      <c r="J3" s="71" t="s">
-        <v>173</v>
+      <c r="J3" s="69" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="4" spans="1:10" s="54" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -4173,11 +4411,11 @@
       <c r="H4" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="I4" s="73">
+      <c r="I4" s="71">
         <v>43</v>
       </c>
-      <c r="J4" s="71" t="s">
-        <v>173</v>
+      <c r="J4" s="69" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="5" spans="1:10" s="54" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -4205,11 +4443,11 @@
       <c r="H5" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="I5" s="73">
+      <c r="I5" s="71">
         <v>1</v>
       </c>
-      <c r="J5" s="71" t="s">
-        <v>173</v>
+      <c r="J5" s="69" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="6" spans="1:10" s="54" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -4237,11 +4475,11 @@
       <c r="H6" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="I6" s="73">
+      <c r="I6" s="71">
         <v>39035</v>
       </c>
-      <c r="J6" s="71" t="s">
-        <v>173</v>
+      <c r="J6" s="69" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="7" spans="1:10" s="54" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -4269,14 +4507,14 @@
       <c r="H7" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="I7" s="73">
+      <c r="I7" s="71">
         <v>63</v>
       </c>
-      <c r="J7" s="71" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" s="54" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="J7" s="69" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" s="54" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="54" t="s">
         <v>40</v>
       </c>
@@ -4301,11 +4539,11 @@
       <c r="H8" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="I8" s="73">
+      <c r="I8" s="71">
         <v>371091</v>
       </c>
-      <c r="J8" s="71" t="s">
-        <v>173</v>
+      <c r="J8" s="69" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="9" spans="1:10" s="54" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -4318,20 +4556,22 @@
       <c r="C9" s="56" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="58" t="s">
-        <v>39</v>
-      </c>
-      <c r="E9" s="63"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="51"/>
+      <c r="D9" s="59" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="81" t="s">
+        <v>274</v>
+      </c>
+      <c r="F9" s="82"/>
+      <c r="G9" s="83"/>
       <c r="H9" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="I9" s="74" t="s">
-        <v>39</v>
-      </c>
-      <c r="J9" s="71" t="s">
-        <v>192</v>
+      <c r="I9" s="72" t="s">
+        <v>39</v>
+      </c>
+      <c r="J9" s="69" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="16" x14ac:dyDescent="0.2">
@@ -4344,20 +4584,22 @@
       <c r="C10" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="E10" s="65"/>
-      <c r="F10" s="26"/>
+      <c r="D10" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="63" t="s">
+        <v>169</v>
+      </c>
+      <c r="F10" s="60"/>
       <c r="G10" s="27"/>
       <c r="H10" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="I10" s="75" t="s">
-        <v>39</v>
-      </c>
-      <c r="J10" s="71" t="s">
-        <v>195</v>
+      <c r="I10" s="73" t="s">
+        <v>39</v>
+      </c>
+      <c r="J10" s="69" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="16" x14ac:dyDescent="0.2">
@@ -4370,20 +4612,20 @@
       <c r="C11" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="E11" s="18"/>
-      <c r="F11" s="26"/>
+      <c r="D11" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" s="61"/>
+      <c r="F11" s="60"/>
       <c r="G11" s="27"/>
       <c r="H11" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="I11" s="75" t="s">
-        <v>39</v>
-      </c>
-      <c r="J11" s="71" t="s">
-        <v>196</v>
+      <c r="I11" s="73" t="s">
+        <v>39</v>
+      </c>
+      <c r="J11" s="69" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="16" x14ac:dyDescent="0.2">
@@ -4396,20 +4638,22 @@
       <c r="C12" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="E12" s="62"/>
-      <c r="F12" s="26"/>
+      <c r="D12" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" s="84" t="s">
+        <v>167</v>
+      </c>
+      <c r="F12" s="60"/>
       <c r="G12" s="27"/>
       <c r="H12" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="I12" s="75" t="s">
-        <v>39</v>
-      </c>
-      <c r="J12" s="71" t="s">
-        <v>177</v>
+      <c r="I12" s="73" t="s">
+        <v>39</v>
+      </c>
+      <c r="J12" s="69" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -4422,20 +4666,22 @@
       <c r="C13" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="D13" s="43" t="s">
-        <v>39</v>
-      </c>
-      <c r="E13" s="44"/>
+      <c r="D13" s="42" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" s="44" t="s">
+        <v>275</v>
+      </c>
       <c r="F13" s="46"/>
       <c r="G13" s="45"/>
       <c r="H13" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="I13" s="75" t="s">
-        <v>39</v>
-      </c>
-      <c r="J13" s="71" t="s">
-        <v>191</v>
+      <c r="I13" s="73" t="s">
+        <v>39</v>
+      </c>
+      <c r="J13" s="69" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="14" spans="1:10" s="39" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -4460,8 +4706,8 @@
       <c r="I14" s="18">
         <v>1</v>
       </c>
-      <c r="J14" s="71" t="s">
-        <v>200</v>
+      <c r="J14" s="69" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="15" spans="1:10" s="54" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -4483,11 +4729,11 @@
       <c r="H15" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="I15" s="73">
+      <c r="I15" s="71">
         <v>5363</v>
       </c>
-      <c r="J15" s="71" t="s">
-        <v>199</v>
+      <c r="J15" s="69" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="16" spans="1:10" s="39" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -4512,8 +4758,8 @@
       <c r="I16" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="J16" s="72" t="s">
-        <v>162</v>
+      <c r="J16" s="70" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="17" spans="1:10" s="39" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -4538,8 +4784,8 @@
       <c r="I17" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="J17" s="72" t="s">
-        <v>162</v>
+      <c r="J17" s="70" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="18" spans="1:10" s="39" customFormat="1" ht="24" x14ac:dyDescent="0.2">
@@ -4561,11 +4807,11 @@
       <c r="H18" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="I18" s="73" t="s">
+      <c r="I18" s="71" t="s">
         <v>158</v>
       </c>
-      <c r="J18" s="71" t="s">
-        <v>234</v>
+      <c r="J18" s="69" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="16" x14ac:dyDescent="0.2">
@@ -4590,8 +4836,8 @@
       <c r="I19" s="18" t="s">
         <v>140</v>
       </c>
-      <c r="J19" s="72" t="s">
-        <v>162</v>
+      <c r="J19" s="70" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="16" x14ac:dyDescent="0.2">
@@ -4616,8 +4862,8 @@
       <c r="I20" s="18" t="s">
         <v>139</v>
       </c>
-      <c r="J20" s="71" t="s">
-        <v>197</v>
+      <c r="J20" s="69" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="21" spans="1:10" s="39" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -4639,11 +4885,11 @@
       <c r="H21" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="I21" s="75" t="s">
-        <v>39</v>
-      </c>
-      <c r="J21" s="72" t="s">
-        <v>162</v>
+      <c r="I21" s="73" t="s">
+        <v>39</v>
+      </c>
+      <c r="J21" s="70" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="16" x14ac:dyDescent="0.2">
@@ -4668,8 +4914,8 @@
       <c r="I22" s="18">
         <v>5200</v>
       </c>
-      <c r="J22" s="71" t="s">
-        <v>198</v>
+      <c r="J22" s="69" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="16" x14ac:dyDescent="0.2">
@@ -4685,7 +4931,7 @@
       <c r="D23" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E23" s="68"/>
+      <c r="E23" s="66"/>
       <c r="F23" s="36"/>
       <c r="G23" s="21"/>
       <c r="H23" s="40" t="s">
@@ -4694,8 +4940,8 @@
       <c r="I23" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="J23" s="71" t="s">
-        <v>237</v>
+      <c r="J23" s="69" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="24" spans="1:10" s="39" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -4720,8 +4966,8 @@
       <c r="I24" s="18">
         <v>0</v>
       </c>
-      <c r="J24" s="71" t="s">
-        <v>201</v>
+      <c r="J24" s="69" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="16" x14ac:dyDescent="0.2">
@@ -4738,16 +4984,20 @@
         <v>39</v>
       </c>
       <c r="E25" s="26"/>
-      <c r="F25" s="36"/>
-      <c r="G25" s="21"/>
+      <c r="F25" s="36" t="s">
+        <v>169</v>
+      </c>
+      <c r="G25" s="21" t="s">
+        <v>267</v>
+      </c>
       <c r="H25" s="40" t="s">
         <v>39</v>
       </c>
       <c r="I25" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="J25" s="71" t="s">
-        <v>202</v>
+      <c r="J25" s="69" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="16" x14ac:dyDescent="0.2">
@@ -4763,17 +5013,21 @@
       <c r="D26" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E26" s="65"/>
-      <c r="F26" s="36"/>
-      <c r="G26" s="21"/>
+      <c r="E26" s="63"/>
+      <c r="F26" s="36" t="s">
+        <v>169</v>
+      </c>
+      <c r="G26" s="21" t="s">
+        <v>268</v>
+      </c>
       <c r="H26" s="40" t="s">
         <v>39</v>
       </c>
       <c r="I26" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="J26" s="71" t="s">
-        <v>203</v>
+      <c r="J26" s="69" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="16" x14ac:dyDescent="0.2">
@@ -4798,8 +5052,8 @@
       <c r="I27" s="18" t="s">
         <v>159</v>
       </c>
-      <c r="J27" s="71" t="s">
-        <v>204</v>
+      <c r="J27" s="69" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="28" spans="1:10" s="39" customFormat="1" ht="24" x14ac:dyDescent="0.2">
@@ -4821,11 +5075,11 @@
       <c r="H28" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="I28" s="75" t="s">
-        <v>39</v>
-      </c>
-      <c r="J28" s="71" t="s">
-        <v>238</v>
+      <c r="I28" s="73" t="s">
+        <v>39</v>
+      </c>
+      <c r="J28" s="69" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="16" x14ac:dyDescent="0.2">
@@ -4841,17 +5095,19 @@
       <c r="D29" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E29" s="26"/>
+      <c r="E29" s="80">
+        <v>44196</v>
+      </c>
       <c r="F29" s="36"/>
       <c r="G29" s="21"/>
       <c r="H29" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="I29" s="76">
+      <c r="I29" s="74">
         <v>44196</v>
       </c>
-      <c r="J29" s="71" t="s">
-        <v>205</v>
+      <c r="J29" s="69" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="16" x14ac:dyDescent="0.2">
@@ -4867,17 +5123,19 @@
       <c r="D30" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E30" s="26"/>
+      <c r="E30" s="80">
+        <v>43831</v>
+      </c>
       <c r="F30" s="36"/>
       <c r="G30" s="21"/>
       <c r="H30" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="I30" s="76">
+      <c r="I30" s="74">
         <v>43831</v>
       </c>
-      <c r="J30" s="71" t="s">
-        <v>206</v>
+      <c r="J30" s="69" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="16" x14ac:dyDescent="0.2">
@@ -4893,7 +5151,7 @@
       <c r="D31" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E31" s="68"/>
+      <c r="E31" s="66"/>
       <c r="F31" s="36"/>
       <c r="G31" s="21"/>
       <c r="H31" s="40" t="s">
@@ -4902,8 +5160,8 @@
       <c r="I31" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="J31" s="72" t="s">
-        <v>162</v>
+      <c r="J31" s="70" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="16" x14ac:dyDescent="0.2">
@@ -4919,17 +5177,21 @@
       <c r="D32" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E32" s="68"/>
-      <c r="F32" s="36"/>
-      <c r="G32" s="21"/>
+      <c r="E32" s="66"/>
+      <c r="F32" s="36" t="s">
+        <v>169</v>
+      </c>
+      <c r="G32" s="21" t="s">
+        <v>244</v>
+      </c>
       <c r="H32" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="I32" s="75" t="s">
-        <v>39</v>
-      </c>
-      <c r="J32" s="71" t="s">
-        <v>207</v>
+      <c r="I32" s="73" t="s">
+        <v>39</v>
+      </c>
+      <c r="J32" s="69" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="16" x14ac:dyDescent="0.2">
@@ -4954,8 +5216,8 @@
       <c r="I33" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="J33" s="72" t="s">
-        <v>162</v>
+      <c r="J33" s="70" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="24" x14ac:dyDescent="0.2">
@@ -4980,8 +5242,8 @@
       <c r="I34" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="J34" s="71" t="s">
-        <v>235</v>
+      <c r="J34" s="69" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="35" spans="1:10" s="54" customFormat="1" ht="24" x14ac:dyDescent="0.2">
@@ -5006,8 +5268,8 @@
       <c r="I35" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="J35" s="71" t="s">
-        <v>236</v>
+      <c r="J35" s="69" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="16" x14ac:dyDescent="0.2">
@@ -5023,17 +5285,17 @@
       <c r="D36" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="E36" s="67"/>
+      <c r="E36" s="65"/>
       <c r="F36" s="36"/>
       <c r="G36" s="21"/>
       <c r="H36" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="I36" s="77">
+      <c r="I36" s="75">
         <v>43874</v>
       </c>
-      <c r="J36" s="71" t="s">
-        <v>208</v>
+      <c r="J36" s="69" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="16" x14ac:dyDescent="0.2">
@@ -5055,11 +5317,11 @@
       <c r="H37" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="I37" s="78">
+      <c r="I37" s="76">
         <v>33187</v>
       </c>
-      <c r="J37" s="72" t="s">
-        <v>162</v>
+      <c r="J37" s="70" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="16" x14ac:dyDescent="0.2">
@@ -5081,11 +5343,11 @@
       <c r="H38" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="I38" s="75" t="s">
-        <v>39</v>
-      </c>
-      <c r="J38" s="71" t="s">
-        <v>209</v>
+      <c r="I38" s="73" t="s">
+        <v>39</v>
+      </c>
+      <c r="J38" s="69" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
@@ -5105,11 +5367,11 @@
       <c r="F39" s="36"/>
       <c r="G39" s="21"/>
       <c r="H39" s="39"/>
-      <c r="I39" s="75" t="s">
-        <v>39</v>
-      </c>
-      <c r="J39" s="71" t="s">
-        <v>210</v>
+      <c r="I39" s="73" t="s">
+        <v>39</v>
+      </c>
+      <c r="J39" s="69" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="24" x14ac:dyDescent="0.2">
@@ -5134,8 +5396,8 @@
       <c r="I40" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="J40" s="71" t="s">
-        <v>239</v>
+      <c r="J40" s="69" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="16" x14ac:dyDescent="0.2">
@@ -5157,11 +5419,11 @@
       <c r="H41" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="I41" s="75" t="s">
-        <v>39</v>
-      </c>
-      <c r="J41" s="72" t="s">
-        <v>162</v>
+      <c r="I41" s="73" t="s">
+        <v>39</v>
+      </c>
+      <c r="J41" s="70" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="16" x14ac:dyDescent="0.2">
@@ -5183,11 +5445,11 @@
       <c r="H42" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="I42" s="75" t="s">
-        <v>39</v>
-      </c>
-      <c r="J42" s="71" t="s">
-        <v>211</v>
+      <c r="I42" s="73" t="s">
+        <v>39</v>
+      </c>
+      <c r="J42" s="69" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="43" spans="1:10" s="54" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -5212,8 +5474,8 @@
       <c r="I43" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="J43" s="72" t="s">
-        <v>162</v>
+      <c r="J43" s="70" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="16" x14ac:dyDescent="0.2">
@@ -5235,11 +5497,11 @@
       <c r="H44" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="I44" s="73" t="s">
+      <c r="I44" s="71" t="s">
         <v>134</v>
       </c>
-      <c r="J44" s="71" t="s">
-        <v>212</v>
+      <c r="J44" s="69" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="16" x14ac:dyDescent="0.2">
@@ -5264,8 +5526,8 @@
       <c r="I45" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="J45" s="71" t="s">
-        <v>213</v>
+      <c r="J45" s="69" t="s">
+        <v>228</v>
       </c>
     </row>
   </sheetData>
@@ -5289,32 +5551,32 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="66"/>
-      <c r="B1" s="66"/>
+      <c r="A1" s="64"/>
+      <c r="B1" s="64"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="66"/>
-      <c r="B2" s="66"/>
+      <c r="A2" s="64"/>
+      <c r="B2" s="64"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="66"/>
-      <c r="B3" s="66"/>
+      <c r="A3" s="64"/>
+      <c r="B3" s="64"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="66"/>
-      <c r="B4" s="66"/>
+      <c r="A4" s="64"/>
+      <c r="B4" s="64"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="66"/>
-      <c r="B5" s="66"/>
+      <c r="A5" s="64"/>
+      <c r="B5" s="64"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="66"/>
-      <c r="B6" s="66"/>
+      <c r="A6" s="64"/>
+      <c r="B6" s="64"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="66"/>
-      <c r="B7" s="66"/>
+      <c r="A7" s="64"/>
+      <c r="B7" s="64"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Texas water rights update.
Texas water rights update.
</commit_message>
<xml_diff>
--- a/Texas/WaterAllocation/TX_Allocation Schema Mapping to WaDE_QA.xlsx
+++ b/Texas/WaterAllocation/TX_Allocation Schema Mapping to WaDE_QA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rjame\Documents\WSWC Documents\MappingStatesDataToWaDE2.0\Texas\WaterAllocation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A74C1D92-8D66-47FB-BBA9-F69D21806A29}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E127D8E1-9B46-46CC-A1B4-0C3C6080FAE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" tabRatio="714" activeTab="3" xr2:uid="{10FC1BAB-5472-410C-A2F0-85DCDF5389F8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" tabRatio="714" activeTab="6" xr2:uid="{10FC1BAB-5472-410C-A2F0-85DCDF5389F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapping Notes" sheetId="10" r:id="rId1"/>
@@ -20,7 +20,6 @@
     <sheet name="WaterSources" sheetId="3" r:id="rId5"/>
     <sheet name="Sites" sheetId="5" r:id="rId6"/>
     <sheet name="AllocationsAmounts_fact" sheetId="7" r:id="rId7"/>
-    <sheet name="BeneficialUseCategory" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1032" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1043" uniqueCount="298">
   <si>
     <t>AllocationAmount</t>
   </si>
@@ -897,8 +896,35 @@
     <t>Current TCEQ data does not tie in very well to water sources.</t>
   </si>
   <si>
+    <t>Notes for mapping to Local QA that need to be changed for Live</t>
+  </si>
+  <si>
+    <t>There are spelling errors in their 'TYPE' field, which we use for SiteType.  Had to pre-procsses to fix this.</t>
+  </si>
+  <si>
+    <t>Had to include some TX specific CVs.SiteType, roughly 30 in total.</t>
+  </si>
+  <si>
+    <t>Kathy Alexander</t>
+  </si>
+  <si>
+    <t>kathy.alexander@tceq.texas.gov</t>
+  </si>
+  <si>
+    <t>Removed special characters from Owner name to help with keyword Search</t>
+  </si>
+  <si>
+    <t>5)</t>
+  </si>
+  <si>
+    <t>Reored owner name for first &amp; last name, better keyword search</t>
+  </si>
+  <si>
+    <t>4)</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve"> Current TCEQ reports water allocation site, but not Amount and Priotity Date.  </t>
+      <t xml:space="preserve">Current TCEQ reports water allocation site, but not Amount and Priotity Date.  </t>
     </r>
     <r>
       <rPr>
@@ -913,19 +939,13 @@
     </r>
   </si>
   <si>
-    <t>Notes for mapping to Local QA that need to be changed for Live</t>
-  </si>
-  <si>
-    <t>There are spelling errors in their 'TYPE' field, which we use for SiteType.  Had to pre-procsses to fix this.</t>
-  </si>
-  <si>
-    <t>Had to include some TX specific CVs.SiteType, roughly 30 in total.</t>
-  </si>
-  <si>
-    <t>Kathy Alexander</t>
-  </si>
-  <si>
-    <t>kathy.alexander@tceq.texas.gov</t>
+    <t>OwnerClassificationCV</t>
+  </si>
+  <si>
+    <t>Army (USA)</t>
+  </si>
+  <si>
+    <t>WSWC defined owner tag.</t>
   </si>
 </sst>
 </file>
@@ -1695,7 +1715,7 @@
     <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1883,9 +1903,6 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="23" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="21" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1964,6 +1981,12 @@
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="42" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -2323,26 +2346,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7154D4B-C952-456C-B506-1C3DB2041E3D}">
   <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView topLeftCell="A6" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.77734375" style="76" customWidth="1"/>
+    <col min="1" max="1" width="13.77734375" style="75" customWidth="1"/>
     <col min="2" max="2" width="79" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="75" t="s">
         <v>273</v>
       </c>
-      <c r="B1" s="81">
+      <c r="B1" s="80">
         <v>43999</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="76" t="s">
+      <c r="A2" s="75" t="s">
         <v>255</v>
       </c>
       <c r="B2" t="s">
@@ -2350,7 +2373,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="76" t="s">
+      <c r="A3" s="75" t="s">
         <v>257</v>
       </c>
       <c r="B3" t="s">
@@ -2358,42 +2381,42 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="76" t="s">
+      <c r="A6" s="75" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="89" t="s">
+      <c r="A7" s="88" t="s">
         <v>280</v>
       </c>
-      <c r="B7" s="66" t="s">
+      <c r="B7" s="65" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="89" t="s">
+      <c r="A8" s="88" t="s">
         <v>281</v>
       </c>
-      <c r="B8" s="66" t="s">
+      <c r="B8" s="65" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="89"/>
+      <c r="A9" s="88"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="89"/>
+      <c r="A10" s="88"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="89"/>
+      <c r="A11" s="88"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="76" t="s">
+      <c r="A12" s="75" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="89" t="s">
+      <c r="A13" s="88" t="s">
         <v>280</v>
       </c>
       <c r="B13" t="s">
@@ -2401,7 +2424,7 @@
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="89" t="s">
+      <c r="A14" s="88" t="s">
         <v>281</v>
       </c>
       <c r="B14" t="s">
@@ -2409,69 +2432,79 @@
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="89" t="s">
+      <c r="A15" s="88" t="s">
         <v>282</v>
       </c>
       <c r="B15" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="88" t="s">
+        <v>293</v>
+      </c>
+      <c r="B16" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="88" t="s">
+        <v>291</v>
+      </c>
+      <c r="B17" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="88"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="88"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="87" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="89"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="89"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="89"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="89"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="88" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="88" t="s">
+        <v>280</v>
+      </c>
+      <c r="B21" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="89" t="s">
-        <v>280</v>
-      </c>
-      <c r="B21" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="88" t="s">
+        <v>281</v>
+      </c>
+      <c r="B22" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="89" t="s">
-        <v>281</v>
-      </c>
-      <c r="B22" t="s">
-        <v>288</v>
-      </c>
-    </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="89"/>
+      <c r="A23" s="88"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="89"/>
+      <c r="A24" s="88"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="89"/>
+      <c r="A25" s="88"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="89"/>
+      <c r="A26" s="88"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" s="89"/>
+      <c r="A27" s="88"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" s="89"/>
+      <c r="A28" s="88"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" s="89"/>
+      <c r="A29" s="88"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" s="89"/>
+      <c r="A30" s="88"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2573,7 +2606,7 @@
       <c r="I3" s="17">
         <v>11</v>
       </c>
-      <c r="J3" s="67" t="s">
+      <c r="J3" s="66" t="s">
         <v>187</v>
       </c>
     </row>
@@ -2605,7 +2638,7 @@
       <c r="I4" s="17" t="s">
         <v>141</v>
       </c>
-      <c r="J4" s="67" t="s">
+      <c r="J4" s="66" t="s">
         <v>206</v>
       </c>
     </row>
@@ -2637,7 +2670,7 @@
       <c r="I5" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="J5" s="67" t="s">
+      <c r="J5" s="66" t="s">
         <v>232</v>
       </c>
     </row>
@@ -2666,10 +2699,10 @@
       <c r="H6" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="I6" s="75">
+      <c r="I6" s="74">
         <v>0.5</v>
       </c>
-      <c r="J6" s="67" t="s">
+      <c r="J6" s="66" t="s">
         <v>189</v>
       </c>
     </row>
@@ -2701,7 +2734,7 @@
       <c r="I7" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="J7" s="67" t="s">
+      <c r="J7" s="66" t="s">
         <v>188</v>
       </c>
     </row>
@@ -2733,7 +2766,7 @@
       <c r="I8" s="20" t="s">
         <v>228</v>
       </c>
-      <c r="J8" s="67" t="s">
+      <c r="J8" s="66" t="s">
         <v>234</v>
       </c>
     </row>
@@ -2763,7 +2796,7 @@
         <v>39</v>
       </c>
       <c r="I9" s="18"/>
-      <c r="J9" s="67" t="s">
+      <c r="J9" s="66" t="s">
         <v>229</v>
       </c>
     </row>
@@ -2795,7 +2828,7 @@
       <c r="I10" s="17" t="s">
         <v>145</v>
       </c>
-      <c r="J10" s="67" t="s">
+      <c r="J10" s="66" t="s">
         <v>186</v>
       </c>
     </row>
@@ -2812,7 +2845,7 @@
       <c r="D11" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E11" s="77" t="s">
+      <c r="E11" s="76" t="s">
         <v>260</v>
       </c>
       <c r="F11" s="20" t="s">
@@ -2827,7 +2860,7 @@
       <c r="I11" s="17" t="s">
         <v>109</v>
       </c>
-      <c r="J11" s="67" t="s">
+      <c r="J11" s="66" t="s">
         <v>190</v>
       </c>
     </row>
@@ -2859,7 +2892,7 @@
       <c r="I12" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="J12" s="67" t="s">
+      <c r="J12" s="66" t="s">
         <v>233</v>
       </c>
     </row>
@@ -2962,7 +2995,7 @@
       <c r="I3" s="17">
         <v>16</v>
       </c>
-      <c r="J3" s="67" t="s">
+      <c r="J3" s="66" t="s">
         <v>187</v>
       </c>
     </row>
@@ -2994,7 +3027,7 @@
       <c r="I4" s="17" t="s">
         <v>142</v>
       </c>
-      <c r="J4" s="67" t="s">
+      <c r="J4" s="66" t="s">
         <v>191</v>
       </c>
     </row>
@@ -3026,7 +3059,7 @@
       <c r="I5" s="17">
         <v>1</v>
       </c>
-      <c r="J5" s="67" t="s">
+      <c r="J5" s="66" t="s">
         <v>192</v>
       </c>
     </row>
@@ -3058,7 +3091,7 @@
       <c r="I6" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="J6" s="67" t="s">
+      <c r="J6" s="66" t="s">
         <v>193</v>
       </c>
     </row>
@@ -3090,7 +3123,7 @@
       <c r="I7" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="J7" s="67" t="s">
+      <c r="J7" s="66" t="s">
         <v>235</v>
       </c>
     </row>
@@ -3122,7 +3155,7 @@
       <c r="I8" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="J8" s="67" t="s">
+      <c r="J8" s="66" t="s">
         <v>236</v>
       </c>
     </row>
@@ -3154,7 +3187,7 @@
       <c r="I9" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="J9" s="67" t="s">
+      <c r="J9" s="66" t="s">
         <v>230</v>
       </c>
     </row>
@@ -3186,7 +3219,7 @@
       <c r="I10" s="17">
         <v>10</v>
       </c>
-      <c r="J10" s="67" t="s">
+      <c r="J10" s="66" t="s">
         <v>194</v>
       </c>
     </row>
@@ -3218,7 +3251,7 @@
       <c r="I11" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="J11" s="67" t="s">
+      <c r="J11" s="66" t="s">
         <v>237</v>
       </c>
     </row>
@@ -3250,7 +3283,7 @@
       <c r="I12" s="17" t="s">
         <v>146</v>
       </c>
-      <c r="J12" s="67" t="s">
+      <c r="J12" s="66" t="s">
         <v>238</v>
       </c>
     </row>
@@ -3282,7 +3315,7 @@
       <c r="I13" s="17" t="s">
         <v>117</v>
       </c>
-      <c r="J13" s="67" t="s">
+      <c r="J13" s="66" t="s">
         <v>231</v>
       </c>
     </row>
@@ -3299,7 +3332,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E8BA2FE-2555-4166-A4DF-0203EE1C77D7}">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
@@ -3385,7 +3418,7 @@
       <c r="I3" s="18">
         <v>1</v>
       </c>
-      <c r="J3" s="67" t="s">
+      <c r="J3" s="66" t="s">
         <v>187</v>
       </c>
     </row>
@@ -3417,7 +3450,7 @@
       <c r="I4" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="J4" s="67" t="s">
+      <c r="J4" s="66" t="s">
         <v>195</v>
       </c>
     </row>
@@ -3434,8 +3467,8 @@
       <c r="D5" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E5" s="90" t="s">
-        <v>290</v>
+      <c r="E5" s="89" t="s">
+        <v>289</v>
       </c>
       <c r="F5" s="20" t="s">
         <v>39</v>
@@ -3449,7 +3482,7 @@
       <c r="I5" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="J5" s="67" t="s">
+      <c r="J5" s="66" t="s">
         <v>196</v>
       </c>
     </row>
@@ -3467,7 +3500,7 @@
         <v>39</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F6" s="20" t="s">
         <v>39</v>
@@ -3481,7 +3514,7 @@
       <c r="I6" s="18" t="s">
         <v>131</v>
       </c>
-      <c r="J6" s="67" t="s">
+      <c r="J6" s="66" t="s">
         <v>197</v>
       </c>
     </row>
@@ -3513,7 +3546,7 @@
       <c r="I7" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="J7" s="67" t="s">
+      <c r="J7" s="66" t="s">
         <v>198</v>
       </c>
     </row>
@@ -3545,7 +3578,7 @@
       <c r="I8" s="18" t="s">
         <v>149</v>
       </c>
-      <c r="J8" s="67" t="s">
+      <c r="J8" s="66" t="s">
         <v>199</v>
       </c>
     </row>
@@ -3577,7 +3610,7 @@
       <c r="I9" s="18" t="s">
         <v>130</v>
       </c>
-      <c r="J9" s="67" t="s">
+      <c r="J9" s="66" t="s">
         <v>200</v>
       </c>
     </row>
@@ -3609,7 +3642,7 @@
       <c r="I10" s="18" t="s">
         <v>150</v>
       </c>
-      <c r="J10" s="67" t="s">
+      <c r="J10" s="66" t="s">
         <v>201</v>
       </c>
     </row>
@@ -3641,7 +3674,7 @@
       <c r="I11" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="J11" s="67" t="s">
+      <c r="J11" s="66" t="s">
         <v>202</v>
       </c>
     </row>
@@ -3673,7 +3706,7 @@
       <c r="I12" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="J12" s="67" t="s">
+      <c r="J12" s="66" t="s">
         <v>203</v>
       </c>
     </row>
@@ -3801,7 +3834,7 @@
       <c r="I3" s="17">
         <v>34658</v>
       </c>
-      <c r="J3" s="67" t="s">
+      <c r="J3" s="66" t="s">
         <v>187</v>
       </c>
     </row>
@@ -3831,7 +3864,7 @@
       <c r="I4" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="J4" s="67" t="s">
+      <c r="J4" s="66" t="s">
         <v>205</v>
       </c>
     </row>
@@ -3861,7 +3894,7 @@
       <c r="I5" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="J5" s="67" t="s">
+      <c r="J5" s="66" t="s">
         <v>179</v>
       </c>
     </row>
@@ -3891,7 +3924,7 @@
       <c r="I6" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="J6" s="67" t="s">
+      <c r="J6" s="66" t="s">
         <v>239</v>
       </c>
     </row>
@@ -3921,7 +3954,7 @@
       <c r="I7" s="17" t="s">
         <v>120</v>
       </c>
-      <c r="J7" s="67" t="s">
+      <c r="J7" s="66" t="s">
         <v>240</v>
       </c>
     </row>
@@ -3951,7 +3984,7 @@
       <c r="I8" s="17" t="s">
         <v>204</v>
       </c>
-      <c r="J8" s="67" t="s">
+      <c r="J8" s="66" t="s">
         <v>207</v>
       </c>
     </row>
@@ -3981,7 +4014,7 @@
       <c r="I9" s="17">
         <v>17839</v>
       </c>
-      <c r="J9" s="67" t="s">
+      <c r="J9" s="66" t="s">
         <v>208</v>
       </c>
     </row>
@@ -4011,7 +4044,7 @@
       <c r="I10" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="J10" s="67" t="s">
+      <c r="J10" s="66" t="s">
         <v>241</v>
       </c>
     </row>
@@ -4037,7 +4070,7 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4120,7 +4153,7 @@
       <c r="I3" s="18">
         <v>39035</v>
       </c>
-      <c r="J3" s="67" t="s">
+      <c r="J3" s="66" t="s">
         <v>177</v>
       </c>
     </row>
@@ -4144,7 +4177,7 @@
       <c r="I4" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="J4" s="67" t="s">
+      <c r="J4" s="66" t="s">
         <v>178</v>
       </c>
     </row>
@@ -4161,7 +4194,7 @@
       <c r="D5" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E5" s="82" t="s">
+      <c r="E5" s="81" t="s">
         <v>119</v>
       </c>
       <c r="F5" s="20" t="s">
@@ -4174,7 +4207,7 @@
       <c r="I5" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="J5" s="67" t="s">
+      <c r="J5" s="66" t="s">
         <v>247</v>
       </c>
     </row>
@@ -4204,7 +4237,7 @@
       <c r="I6" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="J6" s="67" t="s">
+      <c r="J6" s="66" t="s">
         <v>242</v>
       </c>
     </row>
@@ -4234,7 +4267,7 @@
       <c r="I7" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="J7" s="68" t="s">
+      <c r="J7" s="67" t="s">
         <v>175</v>
       </c>
     </row>
@@ -4264,7 +4297,7 @@
       <c r="I8" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="J8" s="67" t="s">
+      <c r="J8" s="66" t="s">
         <v>180</v>
       </c>
     </row>
@@ -4292,7 +4325,7 @@
       </c>
       <c r="H9" s="19"/>
       <c r="I9" s="18"/>
-      <c r="J9" s="67" t="s">
+      <c r="J9" s="66" t="s">
         <v>179</v>
       </c>
     </row>
@@ -4322,7 +4355,7 @@
       <c r="I10" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="J10" s="67" t="s">
+      <c r="J10" s="66" t="s">
         <v>181</v>
       </c>
     </row>
@@ -4352,7 +4385,7 @@
       <c r="I11" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="J11" s="68" t="s">
+      <c r="J11" s="67" t="s">
         <v>175</v>
       </c>
     </row>
@@ -4382,7 +4415,7 @@
       <c r="I12" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="J12" s="68" t="s">
+      <c r="J12" s="67" t="s">
         <v>175</v>
       </c>
     </row>
@@ -4412,7 +4445,7 @@
       <c r="I13" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="J13" s="67" t="s">
+      <c r="J13" s="66" t="s">
         <v>182</v>
       </c>
     </row>
@@ -4442,7 +4475,7 @@
       <c r="I14" s="18">
         <v>-1067.700435</v>
       </c>
-      <c r="J14" s="67" t="s">
+      <c r="J14" s="66" t="s">
         <v>183</v>
       </c>
     </row>
@@ -4472,7 +4505,7 @@
       <c r="I15" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="J15" s="67" t="s">
+      <c r="J15" s="66" t="s">
         <v>244</v>
       </c>
     </row>
@@ -4502,7 +4535,7 @@
       <c r="I16" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="J16" s="67" t="s">
+      <c r="J16" s="66" t="s">
         <v>248</v>
       </c>
     </row>
@@ -4530,7 +4563,7 @@
       <c r="I17" s="18" t="s">
         <v>122</v>
       </c>
-      <c r="J17" s="67" t="s">
+      <c r="J17" s="66" t="s">
         <v>184</v>
       </c>
     </row>
@@ -4560,7 +4593,7 @@
       <c r="I18" s="18">
         <v>3703994</v>
       </c>
-      <c r="J18" s="67" t="s">
+      <c r="J18" s="66" t="s">
         <v>185</v>
       </c>
     </row>
@@ -4590,7 +4623,7 @@
       <c r="I19" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="J19" s="68" t="s">
+      <c r="J19" s="67" t="s">
         <v>175</v>
       </c>
     </row>
@@ -4620,7 +4653,7 @@
       <c r="I20" s="18" t="s">
         <v>123</v>
       </c>
-      <c r="J20" s="67" t="s">
+      <c r="J20" s="66" t="s">
         <v>245</v>
       </c>
     </row>
@@ -4650,7 +4683,7 @@
       <c r="I21" s="18" t="s">
         <v>143</v>
       </c>
-      <c r="J21" s="67" t="s">
+      <c r="J21" s="66" t="s">
         <v>246</v>
       </c>
     </row>
@@ -4680,7 +4713,7 @@
       <c r="I22" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="J22" s="68" t="s">
+      <c r="J22" s="67" t="s">
         <v>175</v>
       </c>
     </row>
@@ -4695,10 +4728,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B91B1FF-D207-4871-B787-27544A9D3030}">
-  <dimension ref="A1:J45"/>
+  <dimension ref="A1:P46"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4771,13 +4804,13 @@
       <c r="E3" s="37"/>
       <c r="F3" s="37"/>
       <c r="G3" s="38"/>
-      <c r="H3" s="83" t="s">
-        <v>39</v>
-      </c>
-      <c r="I3" s="69">
+      <c r="H3" s="82" t="s">
+        <v>39</v>
+      </c>
+      <c r="I3" s="68">
         <v>50004</v>
       </c>
-      <c r="J3" s="67" t="s">
+      <c r="J3" s="66" t="s">
         <v>187</v>
       </c>
     </row>
@@ -4803,13 +4836,13 @@
       <c r="G4" s="52" t="s">
         <v>39</v>
       </c>
-      <c r="H4" s="83" t="s">
-        <v>39</v>
-      </c>
-      <c r="I4" s="69">
+      <c r="H4" s="82" t="s">
+        <v>39</v>
+      </c>
+      <c r="I4" s="68">
         <v>43</v>
       </c>
-      <c r="J4" s="67" t="s">
+      <c r="J4" s="66" t="s">
         <v>187</v>
       </c>
     </row>
@@ -4835,13 +4868,13 @@
       <c r="G5" s="52" t="s">
         <v>39</v>
       </c>
-      <c r="H5" s="83" t="s">
-        <v>39</v>
-      </c>
-      <c r="I5" s="69">
+      <c r="H5" s="82" t="s">
+        <v>39</v>
+      </c>
+      <c r="I5" s="68">
         <v>1</v>
       </c>
-      <c r="J5" s="67" t="s">
+      <c r="J5" s="66" t="s">
         <v>187</v>
       </c>
     </row>
@@ -4867,13 +4900,13 @@
       <c r="G6" s="52" t="s">
         <v>39</v>
       </c>
-      <c r="H6" s="83" t="s">
-        <v>39</v>
-      </c>
-      <c r="I6" s="69">
+      <c r="H6" s="82" t="s">
+        <v>39</v>
+      </c>
+      <c r="I6" s="68">
         <v>39035</v>
       </c>
-      <c r="J6" s="67" t="s">
+      <c r="J6" s="66" t="s">
         <v>187</v>
       </c>
     </row>
@@ -4899,13 +4932,13 @@
       <c r="G7" s="52" t="s">
         <v>39</v>
       </c>
-      <c r="H7" s="83" t="s">
-        <v>39</v>
-      </c>
-      <c r="I7" s="69">
+      <c r="H7" s="82" t="s">
+        <v>39</v>
+      </c>
+      <c r="I7" s="68">
         <v>63</v>
       </c>
-      <c r="J7" s="67" t="s">
+      <c r="J7" s="66" t="s">
         <v>187</v>
       </c>
     </row>
@@ -4931,13 +4964,13 @@
       <c r="G8" s="52" t="s">
         <v>39</v>
       </c>
-      <c r="H8" s="83" t="s">
-        <v>39</v>
-      </c>
-      <c r="I8" s="69">
+      <c r="H8" s="82" t="s">
+        <v>39</v>
+      </c>
+      <c r="I8" s="68">
         <v>371091</v>
       </c>
-      <c r="J8" s="67" t="s">
+      <c r="J8" s="66" t="s">
         <v>187</v>
       </c>
     </row>
@@ -4954,22 +4987,22 @@
       <c r="D9" s="57" t="s">
         <v>39</v>
       </c>
-      <c r="E9" s="87" t="s">
+      <c r="E9" s="86" t="s">
         <v>162</v>
       </c>
-      <c r="F9" s="79" t="s">
-        <v>39</v>
-      </c>
-      <c r="G9" s="80" t="s">
-        <v>39</v>
-      </c>
-      <c r="H9" s="83" t="s">
-        <v>39</v>
-      </c>
-      <c r="I9" s="70" t="s">
-        <v>39</v>
-      </c>
-      <c r="J9" s="67" t="s">
+      <c r="F9" s="78" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" s="79" t="s">
+        <v>39</v>
+      </c>
+      <c r="H9" s="82" t="s">
+        <v>39</v>
+      </c>
+      <c r="I9" s="69" t="s">
+        <v>39</v>
+      </c>
+      <c r="J9" s="66" t="s">
         <v>206</v>
       </c>
     </row>
@@ -4995,13 +5028,13 @@
       <c r="G10" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="H10" s="83" t="s">
-        <v>39</v>
-      </c>
-      <c r="I10" s="71" t="s">
-        <v>39</v>
-      </c>
-      <c r="J10" s="67" t="s">
+      <c r="H10" s="82" t="s">
+        <v>39</v>
+      </c>
+      <c r="I10" s="70" t="s">
+        <v>39</v>
+      </c>
+      <c r="J10" s="66" t="s">
         <v>209</v>
       </c>
     </row>
@@ -5027,13 +5060,13 @@
       <c r="G11" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="H11" s="83" t="s">
-        <v>39</v>
-      </c>
-      <c r="I11" s="71" t="s">
-        <v>39</v>
-      </c>
-      <c r="J11" s="67" t="s">
+      <c r="H11" s="82" t="s">
+        <v>39</v>
+      </c>
+      <c r="I11" s="70" t="s">
+        <v>39</v>
+      </c>
+      <c r="J11" s="66" t="s">
         <v>210</v>
       </c>
     </row>
@@ -5059,13 +5092,13 @@
       <c r="G12" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="H12" s="83" t="s">
-        <v>39</v>
-      </c>
-      <c r="I12" s="71" t="s">
-        <v>39</v>
-      </c>
-      <c r="J12" s="67" t="s">
+      <c r="H12" s="82" t="s">
+        <v>39</v>
+      </c>
+      <c r="I12" s="70" t="s">
+        <v>39</v>
+      </c>
+      <c r="J12" s="66" t="s">
         <v>191</v>
       </c>
     </row>
@@ -5091,13 +5124,13 @@
       <c r="G13" s="44" t="s">
         <v>39</v>
       </c>
-      <c r="H13" s="84" t="s">
+      <c r="H13" s="83" t="s">
         <v>279</v>
       </c>
-      <c r="I13" s="71" t="s">
-        <v>39</v>
-      </c>
-      <c r="J13" s="67" t="s">
+      <c r="I13" s="70" t="s">
+        <v>39</v>
+      </c>
+      <c r="J13" s="66" t="s">
         <v>205</v>
       </c>
     </row>
@@ -5123,13 +5156,13 @@
       <c r="G14" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="H14" s="83" t="s">
+      <c r="H14" s="82" t="s">
         <v>39</v>
       </c>
       <c r="I14" s="18">
         <v>1</v>
       </c>
-      <c r="J14" s="67" t="s">
+      <c r="J14" s="66" t="s">
         <v>214</v>
       </c>
     </row>
@@ -5155,13 +5188,13 @@
       <c r="G15" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="H15" s="83" t="s">
-        <v>39</v>
-      </c>
-      <c r="I15" s="69">
+      <c r="H15" s="82" t="s">
+        <v>39</v>
+      </c>
+      <c r="I15" s="68">
         <v>5363</v>
       </c>
-      <c r="J15" s="67" t="s">
+      <c r="J15" s="66" t="s">
         <v>213</v>
       </c>
     </row>
@@ -5187,13 +5220,13 @@
       <c r="G16" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="H16" s="83" t="s">
+      <c r="H16" s="82" t="s">
         <v>39</v>
       </c>
       <c r="I16" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="J16" s="68" t="s">
+      <c r="J16" s="67" t="s">
         <v>175</v>
       </c>
     </row>
@@ -5219,13 +5252,13 @@
       <c r="G17" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="H17" s="83" t="s">
+      <c r="H17" s="82" t="s">
         <v>39</v>
       </c>
       <c r="I17" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="J17" s="68" t="s">
+      <c r="J17" s="67" t="s">
         <v>175</v>
       </c>
     </row>
@@ -5251,13 +5284,13 @@
       <c r="G18" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="H18" s="83" t="s">
-        <v>39</v>
-      </c>
-      <c r="I18" s="69" t="s">
+      <c r="H18" s="82" t="s">
+        <v>39</v>
+      </c>
+      <c r="I18" s="68" t="s">
         <v>158</v>
       </c>
-      <c r="J18" s="67" t="s">
+      <c r="J18" s="66" t="s">
         <v>249</v>
       </c>
     </row>
@@ -5283,13 +5316,13 @@
       <c r="G19" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="H19" s="83" t="s">
+      <c r="H19" s="82" t="s">
         <v>39</v>
       </c>
       <c r="I19" s="18" t="s">
         <v>140</v>
       </c>
-      <c r="J19" s="68" t="s">
+      <c r="J19" s="67" t="s">
         <v>175</v>
       </c>
     </row>
@@ -5315,13 +5348,13 @@
       <c r="G20" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="H20" s="83" t="s">
+      <c r="H20" s="82" t="s">
         <v>39</v>
       </c>
       <c r="I20" s="18" t="s">
         <v>139</v>
       </c>
-      <c r="J20" s="67" t="s">
+      <c r="J20" s="66" t="s">
         <v>211</v>
       </c>
     </row>
@@ -5347,13 +5380,13 @@
       <c r="G21" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="H21" s="83" t="s">
-        <v>39</v>
-      </c>
-      <c r="I21" s="71" t="s">
-        <v>39</v>
-      </c>
-      <c r="J21" s="68" t="s">
+      <c r="H21" s="82" t="s">
+        <v>39</v>
+      </c>
+      <c r="I21" s="70" t="s">
+        <v>39</v>
+      </c>
+      <c r="J21" s="67" t="s">
         <v>175</v>
       </c>
     </row>
@@ -5379,13 +5412,13 @@
       <c r="G22" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="H22" s="83" t="s">
+      <c r="H22" s="82" t="s">
         <v>39</v>
       </c>
       <c r="I22" s="18">
         <v>5200</v>
       </c>
-      <c r="J22" s="67" t="s">
+      <c r="J22" s="66" t="s">
         <v>212</v>
       </c>
     </row>
@@ -5411,13 +5444,13 @@
       <c r="G23" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="H23" s="83" t="s">
+      <c r="H23" s="82" t="s">
         <v>39</v>
       </c>
       <c r="I23" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="J23" s="67" t="s">
+      <c r="J23" s="66" t="s">
         <v>252</v>
       </c>
     </row>
@@ -5443,13 +5476,13 @@
       <c r="G24" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="H24" s="83" t="s">
+      <c r="H24" s="82" t="s">
         <v>39</v>
       </c>
       <c r="I24" s="18">
         <v>0</v>
       </c>
-      <c r="J24" s="67" t="s">
+      <c r="J24" s="66" t="s">
         <v>215</v>
       </c>
     </row>
@@ -5475,13 +5508,13 @@
       <c r="G25" s="21" t="s">
         <v>264</v>
       </c>
-      <c r="H25" s="83" t="s">
+      <c r="H25" s="82" t="s">
         <v>39</v>
       </c>
       <c r="I25" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="J25" s="67" t="s">
+      <c r="J25" s="66" t="s">
         <v>216</v>
       </c>
     </row>
@@ -5507,13 +5540,13 @@
       <c r="G26" s="21" t="s">
         <v>265</v>
       </c>
-      <c r="H26" s="83" t="s">
+      <c r="H26" s="82" t="s">
         <v>39</v>
       </c>
       <c r="I26" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="J26" s="67" t="s">
+      <c r="J26" s="66" t="s">
         <v>217</v>
       </c>
     </row>
@@ -5530,7 +5563,7 @@
       <c r="D27" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E27" s="86">
+      <c r="E27" s="85">
         <v>44005</v>
       </c>
       <c r="F27" s="36" t="s">
@@ -5539,13 +5572,13 @@
       <c r="G27" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="H27" s="84" t="s">
+      <c r="H27" s="83" t="s">
         <v>274</v>
       </c>
       <c r="I27" s="18" t="s">
         <v>159</v>
       </c>
-      <c r="J27" s="67" t="s">
+      <c r="J27" s="66" t="s">
         <v>218</v>
       </c>
     </row>
@@ -5571,13 +5604,13 @@
       <c r="G28" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="H28" s="83" t="s">
-        <v>39</v>
-      </c>
-      <c r="I28" s="71" t="s">
-        <v>39</v>
-      </c>
-      <c r="J28" s="67" t="s">
+      <c r="H28" s="82" t="s">
+        <v>39</v>
+      </c>
+      <c r="I28" s="70" t="s">
+        <v>39</v>
+      </c>
+      <c r="J28" s="66" t="s">
         <v>253</v>
       </c>
     </row>
@@ -5594,7 +5627,7 @@
       <c r="D29" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E29" s="78">
+      <c r="E29" s="77">
         <v>44196</v>
       </c>
       <c r="F29" s="36" t="s">
@@ -5603,13 +5636,13 @@
       <c r="G29" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="H29" s="83" t="s">
-        <v>39</v>
-      </c>
-      <c r="I29" s="72">
+      <c r="H29" s="82" t="s">
+        <v>39</v>
+      </c>
+      <c r="I29" s="71">
         <v>44196</v>
       </c>
-      <c r="J29" s="67" t="s">
+      <c r="J29" s="66" t="s">
         <v>219</v>
       </c>
     </row>
@@ -5626,7 +5659,7 @@
       <c r="D30" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E30" s="78">
+      <c r="E30" s="77">
         <v>43831</v>
       </c>
       <c r="F30" s="36" t="s">
@@ -5635,13 +5668,13 @@
       <c r="G30" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="H30" s="83" t="s">
-        <v>39</v>
-      </c>
-      <c r="I30" s="72">
+      <c r="H30" s="82" t="s">
+        <v>39</v>
+      </c>
+      <c r="I30" s="71">
         <v>43831</v>
       </c>
-      <c r="J30" s="67" t="s">
+      <c r="J30" s="66" t="s">
         <v>220</v>
       </c>
     </row>
@@ -5658,20 +5691,20 @@
       <c r="D31" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E31" s="65"/>
+      <c r="E31" s="64"/>
       <c r="F31" s="36" t="s">
         <v>39</v>
       </c>
       <c r="G31" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="H31" s="83" t="s">
+      <c r="H31" s="82" t="s">
         <v>39</v>
       </c>
       <c r="I31" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="J31" s="68" t="s">
+      <c r="J31" s="67" t="s">
         <v>175</v>
       </c>
     </row>
@@ -5697,17 +5730,17 @@
       <c r="G32" s="21" t="s">
         <v>243</v>
       </c>
-      <c r="H32" s="83" t="s">
-        <v>39</v>
-      </c>
-      <c r="I32" s="71" t="s">
-        <v>39</v>
-      </c>
-      <c r="J32" s="67" t="s">
+      <c r="H32" s="82" t="s">
+        <v>39</v>
+      </c>
+      <c r="I32" s="70" t="s">
+        <v>39</v>
+      </c>
+      <c r="J32" s="66" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>103</v>
       </c>
@@ -5729,17 +5762,17 @@
       <c r="G33" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="H33" s="83" t="s">
+      <c r="H33" s="82" t="s">
         <v>39</v>
       </c>
       <c r="I33" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="J33" s="68" t="s">
+      <c r="J33" s="67" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>100</v>
       </c>
@@ -5761,17 +5794,17 @@
       <c r="G34" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="H34" s="83" t="s">
+      <c r="H34" s="82" t="s">
         <v>39</v>
       </c>
       <c r="I34" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="J34" s="67" t="s">
+      <c r="J34" s="66" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="35" spans="1:10" s="53" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:16" s="53" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>102</v>
       </c>
@@ -5793,17 +5826,17 @@
       <c r="G35" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="H35" s="83" t="s">
+      <c r="H35" s="82" t="s">
         <v>39</v>
       </c>
       <c r="I35" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="J35" s="67" t="s">
+      <c r="J35" s="66" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A36" s="53" t="s">
         <v>157</v>
       </c>
@@ -5816,7 +5849,7 @@
       <c r="D36" s="57" t="s">
         <v>39</v>
       </c>
-      <c r="E36" s="64">
+      <c r="E36" s="63">
         <v>44005</v>
       </c>
       <c r="F36" s="36" t="s">
@@ -5825,17 +5858,17 @@
       <c r="G36" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="H36" s="83" t="s">
-        <v>39</v>
-      </c>
-      <c r="I36" s="73">
+      <c r="H36" s="82" t="s">
+        <v>39</v>
+      </c>
+      <c r="I36" s="72">
         <v>43874</v>
       </c>
-      <c r="J36" s="67" t="s">
+      <c r="J36" s="66" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>83</v>
       </c>
@@ -5857,17 +5890,17 @@
       <c r="G37" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="H37" s="83" t="s">
-        <v>39</v>
-      </c>
-      <c r="I37" s="74">
+      <c r="H37" s="82" t="s">
+        <v>39</v>
+      </c>
+      <c r="I37" s="73">
         <v>33187</v>
       </c>
-      <c r="J37" s="68" t="s">
+      <c r="J37" s="67" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
         <v>92</v>
       </c>
@@ -5889,17 +5922,17 @@
       <c r="G38" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="H38" s="83" t="s">
-        <v>39</v>
-      </c>
-      <c r="I38" s="71" t="s">
-        <v>39</v>
-      </c>
-      <c r="J38" s="67" t="s">
+      <c r="H38" s="82" t="s">
+        <v>39</v>
+      </c>
+      <c r="I38" s="70" t="s">
+        <v>39</v>
+      </c>
+      <c r="J38" s="66" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>93</v>
       </c>
@@ -5921,15 +5954,15 @@
       <c r="G39" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="H39" s="85"/>
-      <c r="I39" s="71" t="s">
-        <v>39</v>
-      </c>
-      <c r="J39" s="67" t="s">
+      <c r="H39" s="84"/>
+      <c r="I39" s="70" t="s">
+        <v>39</v>
+      </c>
+      <c r="J39" s="66" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
         <v>101</v>
       </c>
@@ -5951,19 +5984,19 @@
       <c r="G40" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="H40" s="83" t="s">
+      <c r="H40" s="82" t="s">
         <v>39</v>
       </c>
       <c r="I40" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="J40" s="67" t="s">
+      <c r="J40" s="66" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:16" s="53" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
-        <v>98</v>
+        <v>295</v>
       </c>
       <c r="B41" s="6" t="s">
         <v>35</v>
@@ -5971,34 +6004,34 @@
       <c r="C41" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D41" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="E41" s="26" t="s">
-        <v>164</v>
-      </c>
-      <c r="F41" s="36" t="s">
-        <v>39</v>
-      </c>
-      <c r="G41" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="H41" s="83" t="s">
-        <v>39</v>
-      </c>
-      <c r="I41" s="71" t="s">
-        <v>39</v>
-      </c>
-      <c r="J41" s="68" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D41" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="90"/>
+      <c r="H41" s="91" t="s">
+        <v>39</v>
+      </c>
+      <c r="I41" s="70" t="s">
+        <v>296</v>
+      </c>
+      <c r="J41" s="66" t="s">
+        <v>297</v>
+      </c>
+      <c r="K41" s="5"/>
+      <c r="L41" s="5"/>
+      <c r="M41" s="5"/>
+      <c r="N41" s="5"/>
+      <c r="O41" s="5"/>
+      <c r="P41" s="5"/>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C42" s="6" t="s">
         <v>19</v>
@@ -6015,28 +6048,28 @@
       <c r="G42" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="H42" s="83" t="s">
-        <v>39</v>
-      </c>
-      <c r="I42" s="71" t="s">
+      <c r="H42" s="82" t="s">
+        <v>39</v>
+      </c>
+      <c r="I42" s="70" t="s">
         <v>39</v>
       </c>
       <c r="J42" s="67" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" s="53" customFormat="1" x14ac:dyDescent="0.3">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="C43" s="6" t="s">
         <v>19</v>
       </c>
       <c r="D43" s="10" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="E43" s="26" t="s">
         <v>164</v>
@@ -6047,27 +6080,27 @@
       <c r="G43" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="H43" s="83" t="s">
-        <v>39</v>
-      </c>
-      <c r="I43" s="18" t="s">
-        <v>135</v>
-      </c>
-      <c r="J43" s="68" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A44" s="53" t="s">
-        <v>151</v>
-      </c>
-      <c r="B44" s="54" t="s">
-        <v>107</v>
-      </c>
-      <c r="C44" s="55" t="s">
+      <c r="H43" s="82" t="s">
+        <v>39</v>
+      </c>
+      <c r="I43" s="70" t="s">
+        <v>39</v>
+      </c>
+      <c r="J43" s="66" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" s="53" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C44" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D44" s="57" t="s">
+      <c r="D44" s="10" t="s">
         <v>21</v>
       </c>
       <c r="E44" s="26" t="s">
@@ -6079,28 +6112,28 @@
       <c r="G44" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="H44" s="83" t="s">
-        <v>39</v>
-      </c>
-      <c r="I44" s="69" t="s">
-        <v>134</v>
+      <c r="H44" s="82" t="s">
+        <v>39</v>
+      </c>
+      <c r="I44" s="18" t="s">
+        <v>135</v>
       </c>
       <c r="J44" s="67" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A45" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="B45" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C45" s="6" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A45" s="53" t="s">
+        <v>151</v>
+      </c>
+      <c r="B45" s="54" t="s">
+        <v>107</v>
+      </c>
+      <c r="C45" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="D45" s="10" t="s">
-        <v>39</v>
+      <c r="D45" s="57" t="s">
+        <v>21</v>
       </c>
       <c r="E45" s="26" t="s">
         <v>164</v>
@@ -6111,65 +6144,54 @@
       <c r="G45" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="H45" s="83" t="s">
-        <v>39</v>
-      </c>
-      <c r="I45" s="18" t="s">
+      <c r="H45" s="82" t="s">
+        <v>39</v>
+      </c>
+      <c r="I45" s="68" t="s">
+        <v>134</v>
+      </c>
+      <c r="J45" s="66" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A46" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D46" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E46" s="26" t="s">
+        <v>164</v>
+      </c>
+      <c r="F46" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="G46" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="H46" s="82" t="s">
+        <v>39</v>
+      </c>
+      <c r="I46" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="J45" s="67" t="s">
+      <c r="J46" s="66" t="s">
         <v>227</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A14:J45">
-    <sortCondition ref="A14:A45"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A14:J46">
+    <sortCondition ref="A14:A46"/>
   </sortState>
   <phoneticPr fontId="25" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37A68CD9-E6C8-4C1E-8A36-F76F66BA5935}">
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L27" sqref="L27"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="63"/>
-      <c r="B1" s="63"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="63"/>
-      <c r="B2" s="63"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="63"/>
-      <c r="B3" s="63"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="63"/>
-      <c r="B4" s="63"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="63"/>
-      <c r="B5" s="63"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="63"/>
-      <c r="B6" s="63"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="63"/>
-      <c r="B7" s="63"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>